<commit_message>
ym calculate eff by price
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>sku</t>
   </si>
@@ -38,33 +38,6 @@
   </si>
   <si>
     <t>МГ/КГ</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>Эмаль ПРЕСТИЖ алкидная глянцевая, оранжевый, 425 мл</t>
-  </si>
-  <si>
-    <t>350</t>
-  </si>
-  <si>
-    <t>423</t>
-  </si>
-  <si>
-    <t>МГ</t>
-  </si>
-  <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>Эмаль ПРЕСТИЖ алкидная глянцевая, огненно-красный, 425 мл</t>
-  </si>
-  <si>
-    <t>1250</t>
-  </si>
-  <si>
-    <t>525</t>
   </si>
 </sst>
 </file>
@@ -441,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -471,58 +444,6 @@
       </c>
       <c r="I1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>-0.48120567375886525</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2">
-        <v>127.05</v>
-      </c>
-      <c r="H2">
-        <v>3.5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3">
-        <v>1.0023809523809524</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3">
-        <v>186.25</v>
-      </c>
-      <c r="H3">
-        <v>12.5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>